<commit_message>
Improve the emial's forrmat following the Varrun Gupta’s suggestion.
</commit_message>
<xml_diff>
--- a/WebCapture/WebCapture/DevDiv Dogfooding By M2.xlsx
+++ b/WebCapture/WebCapture/DevDiv Dogfooding By M2.xlsx
@@ -409,7 +409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,54 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Alex Chi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Alex Chi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alex Chi</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alex Chi</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Imporove the format following the Ritesh Parikh <Ritesh.Parikh@microsoft.com> suggestion
</commit_message>
<xml_diff>
--- a/WebCapture/WebCapture/DevDiv Dogfooding By M2.xlsx
+++ b/WebCapture/WebCapture/DevDiv Dogfooding By M2.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="2295" yWindow="2295"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="2295" yWindow="2295"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="21-09-28" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="21-09-29" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -50,7 +50,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
@@ -393,13 +393,14 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -409,13 +410,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="56.140625"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -432,76 +436,545 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Anirudh Garg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>18%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Anson Horton</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>77%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Anthony Cangialosi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>80%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Art Leonard</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>53%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Barry Tang</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>90%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Alex Chi</t>
+          <t>Ulzii Luvsanbat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>58%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bogdan Mihalcea</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>81%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Brandon Bynum</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Chuck Weininger</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dan Moseley</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>61%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Donald Drake</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>72%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Fatima Ijaz</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>42%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Galin Iliev</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Gearard Boland</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Greg Arnits</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Graham Wheeler</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Heather Arbon</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Jeff Schwartz</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>31%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Jonathan Carter</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kai Maetzel</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Kevin Pilch</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Luis Aguilera-Steinert</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Lubo Birov</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>72%</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Mandy Whaley</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>33%</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Manish Jayaswal</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>97%</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Marek Safar</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mayuri Diwan</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Mohammed Abdul Rawoof</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Neeraja Singireddy</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Paul Kuklinski</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>83%</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Paul Chapman</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>33%</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Pavel Feldman</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Qing Ye</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Russell Hadley</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Rui Sun</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Sarika Calla</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>27%</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Samer Alameer</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>28%</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Shawn Rothlisberger</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Svetlana Kofman</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>77%</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Srivatsn Narayanan</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Stefan Schackow</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Sumit Gulwani</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Yuval Mazor</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Zhen Jiao</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16%</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Zhishou Zhang</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>12%</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>